<commit_message>
Working on client ng application
</commit_message>
<xml_diff>
--- a/FamilyFinanceClientApp/User interface schema.xlsx
+++ b/FamilyFinanceClientApp/User interface schema.xlsx
@@ -95,9 +95,6 @@
     <t>Итог</t>
   </si>
   <si>
-    <t>Лепешка</t>
-  </si>
-  <si>
     <t>list</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Запоминать последний выбор</t>
+  </si>
+  <si>
+    <t>Хлеб</t>
   </si>
 </sst>
 </file>
@@ -466,69 +466,69 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -864,7 +864,7 @@
   <dimension ref="B1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,46 +883,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="23"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="26"/>
     </row>
     <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="25"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="28"/>
     </row>
     <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
@@ -945,15 +945,15 @@
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="C5" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="37"/>
+      <c r="H5" s="40"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -962,21 +962,21 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="28"/>
+      <c r="H6" s="31"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="26"/>
+      <c r="M6" s="29"/>
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
@@ -997,11 +997,11 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
@@ -1023,19 +1023,19 @@
       <c r="L8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="10" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G9" s="10">
         <v>4000</v>
@@ -1056,16 +1056,16 @@
         <v>17</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1079,9 +1079,9 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1095,9 +1095,9 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1111,9 +1111,9 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1127,9 +1127,9 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1143,9 +1143,9 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -1159,9 +1159,9 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -1175,9 +1175,9 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1191,9 +1191,9 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -1207,9 +1207,9 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -1223,9 +1223,9 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
@@ -1239,9 +1239,9 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -1255,9 +1255,9 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -1271,9 +1271,9 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -1287,9 +1287,9 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -1303,9 +1303,9 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -1319,9 +1319,9 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -1335,11 +1335,11 @@
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="34"/>
       <c r="F27" s="13">
         <v>1</v>
       </c>
@@ -1386,12 +1386,12 @@
     </row>
     <row r="32" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J32" s="4"/>
-      <c r="K32" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
+      <c r="K32" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
       <c r="O32" s="6"/>
     </row>
     <row r="33" spans="10:15" x14ac:dyDescent="0.3">
@@ -1416,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
@@ -1436,10 +1436,10 @@
         <v>7</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M37" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="6"/>
@@ -1458,13 +1458,13 @@
         <v>8</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O39" s="6"/>
     </row>
@@ -1482,7 +1482,7 @@
         <v>15</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
@@ -1498,11 +1498,11 @@
     </row>
     <row r="43" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J43" s="4"/>
-      <c r="K43" s="39" t="s">
+      <c r="K43" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="L43" s="39" t="s">
-        <v>27</v>
+      <c r="L43" s="42" t="s">
+        <v>26</v>
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -1510,16 +1510,16 @@
     </row>
     <row r="44" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J44" s="4"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="O44" s="6"/>
     </row>
     <row r="45" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J45" s="4"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="6"/>
@@ -1535,10 +1535,10 @@
     <row r="47" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J47" s="4"/>
       <c r="K47" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L47" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="L47" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="O47" s="6"/>
     </row>

</xml_diff>